<commit_message>
Added party name to container and implemented import and export
</commit_message>
<xml_diff>
--- a/HK/Content/ExcelTemplates/import-template.xlsx
+++ b/HK/Content/ExcelTemplates/import-template.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>BuyerName</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>ExporterID</t>
+  </si>
+  <si>
+    <t>PartyName</t>
   </si>
 </sst>
 </file>
@@ -147,7 +150,19 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -158,10 +173,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K74" totalsRowShown="0">
-  <autoFilter ref="A1:K74"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L74" totalsRowShown="0">
+  <autoFilter ref="A1:L74"/>
+  <tableColumns count="12">
     <tableColumn id="1" name="BuyerName"/>
+    <tableColumn id="12" name="PartyName" dataDxfId="0"/>
     <tableColumn id="2" name="CartonNumber"/>
     <tableColumn id="3" name="ProductBuyerName"/>
     <tableColumn id="4" name="Quantity"/>
@@ -462,63 +478,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K90"/>
+  <dimension ref="A1:L90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" customWidth="1"/>
-    <col min="9" max="9" width="21" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" customWidth="1"/>
-    <col min="11" max="11" width="17" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="27" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="10" max="10" width="21" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -530,8 +550,9 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="2"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -543,8 +564,9 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -556,8 +578,9 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -569,8 +592,9 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -582,8 +606,9 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -595,8 +620,9 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -608,8 +634,9 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -621,8 +648,9 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -634,8 +662,9 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -647,8 +676,9 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -660,8 +690,9 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -673,8 +704,9 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -686,8 +718,9 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -699,8 +732,9 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -712,8 +746,9 @@
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -725,8 +760,9 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -738,8 +774,9 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -751,8 +788,9 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -764,8 +802,9 @@
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20" s="2"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -777,8 +816,9 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21" s="2"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -790,8 +830,9 @@
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22" s="2"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -803,8 +844,9 @@
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23" s="2"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -816,8 +858,9 @@
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24" s="2"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -829,8 +872,9 @@
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -842,8 +886,9 @@
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26" s="2"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -855,8 +900,9 @@
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27" s="2"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -868,8 +914,9 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L28" s="2"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -881,8 +928,9 @@
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L29" s="2"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -894,8 +942,9 @@
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L30" s="2"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -907,8 +956,9 @@
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L31" s="2"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -920,8 +970,9 @@
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L32" s="2"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -933,8 +984,9 @@
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L33" s="2"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -946,8 +998,9 @@
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L34" s="2"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -959,8 +1012,9 @@
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L35" s="2"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -972,8 +1026,9 @@
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L36" s="2"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -985,8 +1040,9 @@
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L37" s="2"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -998,8 +1054,9 @@
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L38" s="2"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -1011,8 +1068,9 @@
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L39" s="2"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -1024,8 +1082,9 @@
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L40" s="2"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1037,8 +1096,9 @@
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L41" s="2"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -1050,8 +1110,9 @@
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L42" s="2"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -1063,8 +1124,9 @@
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L43" s="2"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -1076,8 +1138,9 @@
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L44" s="2"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -1089,8 +1152,9 @@
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L45" s="2"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1102,8 +1166,9 @@
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L46" s="2"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -1115,8 +1180,9 @@
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L47" s="2"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -1128,8 +1194,9 @@
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L48" s="2"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -1141,8 +1208,9 @@
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L49" s="2"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -1154,8 +1222,9 @@
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L50" s="2"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -1167,8 +1236,9 @@
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L51" s="2"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -1180,8 +1250,9 @@
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L52" s="2"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -1193,8 +1264,9 @@
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L53" s="2"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -1206,8 +1278,9 @@
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L54" s="2"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -1219,8 +1292,9 @@
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L55" s="2"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -1232,8 +1306,9 @@
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L56" s="2"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -1245,8 +1320,9 @@
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
       <c r="K57" s="2"/>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L57" s="2"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -1258,8 +1334,9 @@
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
       <c r="K58" s="2"/>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L58" s="2"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -1271,8 +1348,9 @@
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
       <c r="K59" s="2"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L59" s="2"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -1284,8 +1362,9 @@
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L60" s="2"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -1297,8 +1376,9 @@
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L61" s="2"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -1310,8 +1390,9 @@
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L62" s="2"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -1323,8 +1404,9 @@
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L63" s="2"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -1336,8 +1418,9 @@
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L64" s="2"/>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -1349,8 +1432,9 @@
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
       <c r="K65" s="2"/>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L65" s="2"/>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -1362,8 +1446,9 @@
       <c r="I66" s="2"/>
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L66" s="2"/>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -1375,8 +1460,9 @@
       <c r="I67" s="2"/>
       <c r="J67" s="2"/>
       <c r="K67" s="2"/>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L67" s="2"/>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -1388,8 +1474,9 @@
       <c r="I68" s="2"/>
       <c r="J68" s="2"/>
       <c r="K68" s="2"/>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L68" s="2"/>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -1401,8 +1488,9 @@
       <c r="I69" s="2"/>
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L69" s="2"/>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -1414,8 +1502,9 @@
       <c r="I70" s="2"/>
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L70" s="2"/>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -1427,8 +1516,9 @@
       <c r="I71" s="2"/>
       <c r="J71" s="2"/>
       <c r="K71" s="2"/>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L71" s="2"/>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -1440,8 +1530,9 @@
       <c r="I72" s="2"/>
       <c r="J72" s="2"/>
       <c r="K72" s="2"/>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L72" s="2"/>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -1453,8 +1544,9 @@
       <c r="I73" s="2"/>
       <c r="J73" s="2"/>
       <c r="K73" s="2"/>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L73" s="2"/>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -1466,8 +1558,9 @@
       <c r="I74" s="2"/>
       <c r="J74" s="2"/>
       <c r="K74" s="2"/>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L74" s="2"/>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -1479,8 +1572,9 @@
       <c r="I75" s="2"/>
       <c r="J75" s="2"/>
       <c r="K75" s="2"/>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L75" s="2"/>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -1492,8 +1586,9 @@
       <c r="I76" s="2"/>
       <c r="J76" s="2"/>
       <c r="K76" s="2"/>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L76" s="2"/>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -1505,8 +1600,9 @@
       <c r="I77" s="2"/>
       <c r="J77" s="2"/>
       <c r="K77" s="2"/>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L77" s="2"/>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -1518,8 +1614,9 @@
       <c r="I78" s="2"/>
       <c r="J78" s="2"/>
       <c r="K78" s="2"/>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L78" s="2"/>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -1531,8 +1628,9 @@
       <c r="I79" s="2"/>
       <c r="J79" s="2"/>
       <c r="K79" s="2"/>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L79" s="2"/>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -1544,8 +1642,9 @@
       <c r="I80" s="2"/>
       <c r="J80" s="2"/>
       <c r="K80" s="2"/>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L80" s="2"/>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -1557,8 +1656,9 @@
       <c r="I81" s="2"/>
       <c r="J81" s="2"/>
       <c r="K81" s="2"/>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L81" s="2"/>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -1570,8 +1670,9 @@
       <c r="I82" s="2"/>
       <c r="J82" s="2"/>
       <c r="K82" s="2"/>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L82" s="2"/>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -1583,8 +1684,9 @@
       <c r="I83" s="2"/>
       <c r="J83" s="2"/>
       <c r="K83" s="2"/>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L83" s="2"/>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -1596,8 +1698,9 @@
       <c r="I84" s="2"/>
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L84" s="2"/>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -1609,8 +1712,9 @@
       <c r="I85" s="2"/>
       <c r="J85" s="2"/>
       <c r="K85" s="2"/>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L85" s="2"/>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -1622,8 +1726,9 @@
       <c r="I86" s="2"/>
       <c r="J86" s="2"/>
       <c r="K86" s="2"/>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L86" s="2"/>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -1635,8 +1740,9 @@
       <c r="I87" s="2"/>
       <c r="J87" s="2"/>
       <c r="K87" s="2"/>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L87" s="2"/>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -1648,8 +1754,9 @@
       <c r="I88" s="2"/>
       <c r="J88" s="2"/>
       <c r="K88" s="2"/>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L88" s="2"/>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -1661,8 +1768,9 @@
       <c r="I89" s="2"/>
       <c r="J89" s="2"/>
       <c r="K89" s="2"/>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L89" s="2"/>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -1674,6 +1782,7 @@
       <c r="I90" s="2"/>
       <c r="J90" s="2"/>
       <c r="K90" s="2"/>
+      <c r="L90" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>